<commit_message>
aggiornata colonna "razionale applicabilita" e completati i test mancanti
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/V.6.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/V.6.0.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbettero\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.9\condivisa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1316A8-07C2-4EE0-97E2-53713831AC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A172891-BD8F-4CCC-8A07-3A078CCA9010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="495" windowWidth="26970" windowHeight="14895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="173">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -734,6 +734,57 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>"Il servizio di validazione non risponde"</t>
+  </si>
+  <si>
+    <t>l'operazione deve essere ritentata successivamente</t>
+  </si>
+  <si>
+    <t>campi non gestiti dall'applicazione</t>
+  </si>
+  <si>
+    <t>caso non gestito dall'applicazione</t>
+  </si>
+  <si>
+    <t>caso non possibile: il CF viene sanificato PRIMA dell'invio della LDO</t>
+  </si>
+  <si>
+    <t>caso non possibile: il Comune Residenza è un dato obbligatorio che non permette l'inserimento della cartella</t>
+  </si>
+  <si>
+    <t>caso non possibile: il nome è campo obbligatorio in assenza del quale non è impossibile l'inserimento di una cartella</t>
+  </si>
+  <si>
+    <t>caso non possibile: il sesso è campo obbligatorio e con valori bloccati, in assenza del quale non è impossibile l'inserimento di una cartella</t>
+  </si>
+  <si>
+    <t>caso non possibile: i campi "condizioni del paziente" e "diagnosi di dimissione" sono obbligatori e la LDO non può essere inviata in assenza di questi</t>
+  </si>
+  <si>
+    <t>caso non possibile: il "decorso ospedaliero" è campo obbligatorio, la LDO non può essere inviata in assenza di questo</t>
+  </si>
+  <si>
+    <t>campo non gestito dall'applicazione</t>
+  </si>
+  <si>
+    <t>caso non possibile: le diagnosi sono selezionate dal dizionario ICD e non possono essere scritte manualmente</t>
+  </si>
+  <si>
+    <t>36544e02119009fa</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>Campo token JWT non valido: Il campo purpose_of_use non è valorizzato</t>
+  </si>
+  <si>
+    <t>503493eb4be71fdf</t>
+  </si>
+  <si>
+    <t>Campo token JWT non valido: Il campo action_id non è corretto</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1168,6 +1219,9 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1190,6 +1244,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3655,7 +3715,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3664,10 +3724,13 @@
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" customWidth="1"/>
-    <col min="6" max="9" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="61.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="9" width="33.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
-    <col min="11" max="15" width="36.42578125" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" style="34" customWidth="1"/>
+    <col min="12" max="15" width="36.42578125" customWidth="1"/>
     <col min="16" max="16" width="27.140625" customWidth="1"/>
     <col min="17" max="17" width="33.140625" customWidth="1"/>
     <col min="18" max="18" width="36.42578125" customWidth="1"/>
@@ -3693,14 +3756,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3718,14 +3781,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="38"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3743,12 +3806,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="46" t="s">
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3767,12 +3830,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="38"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3790,8 +3853,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -3829,7 +3892,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="14.25" customHeight="1">
+    <row r="8" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -3931,7 +3994,9 @@
       <c r="J10" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="34" t="s">
+        <v>158</v>
+      </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
@@ -3967,7 +4032,9 @@
       <c r="J11" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="34" t="s">
+        <v>158</v>
+      </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
@@ -4003,7 +4070,9 @@
       <c r="J12" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="34" t="s">
+        <v>158</v>
+      </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
@@ -4039,7 +4108,9 @@
       <c r="J13" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K13" s="25"/>
+      <c r="K13" s="34" t="s">
+        <v>158</v>
+      </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
@@ -4052,7 +4123,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="14" spans="1:20" ht="147.75" customHeight="1" thickBot="1">
       <c r="A14" s="20">
         <v>29</v>
       </c>
@@ -4068,27 +4139,43 @@
       <c r="E14" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25" t="s">
-        <v>110</v>
+      <c r="F14" s="23">
+        <v>45189</v>
+      </c>
+      <c r="G14" s="24">
+        <v>45189.352951388886</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J14" s="48" t="s">
+        <v>54</v>
       </c>
       <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
+      <c r="L14" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="48" t="s">
+        <v>170</v>
+      </c>
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
+      <c r="Q14" s="48" t="s">
+        <v>108</v>
+      </c>
       <c r="R14" s="26"/>
       <c r="S14" s="27"/>
       <c r="T14" s="28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="15" spans="1:20" ht="102.75" customHeight="1" thickBot="1">
       <c r="A15" s="20">
         <v>37</v>
       </c>
@@ -4101,30 +4188,46 @@
       <c r="D15" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="25" t="s">
-        <v>110</v>
+      <c r="F15" s="23">
+        <v>45189</v>
+      </c>
+      <c r="G15" s="24">
+        <v>45189.356828703705</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" s="48" t="s">
+        <v>54</v>
       </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
+      <c r="L15" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15" s="48" t="s">
+        <v>172</v>
+      </c>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
+      <c r="Q15" s="48" t="s">
+        <v>108</v>
+      </c>
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
       <c r="T15" s="28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="16" spans="1:20" ht="122.25" customHeight="1" thickBot="1">
       <c r="A16" s="20">
         <v>45</v>
       </c>
@@ -4145,15 +4248,27 @@
       <c r="H16" s="24"/>
       <c r="I16" s="24"/>
       <c r="J16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="O16" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="25"/>
+      <c r="P16" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q16" s="48" t="s">
+        <v>108</v>
+      </c>
       <c r="R16" s="26" t="s">
         <v>54</v>
       </c>
@@ -4185,7 +4300,9 @@
       <c r="J17" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K17" s="25"/>
+      <c r="K17" s="25" t="s">
+        <v>159</v>
+      </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
@@ -4198,7 +4315,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="18" spans="1:20" ht="30" customHeight="1" thickBot="1">
       <c r="A18" s="20">
         <v>64</v>
       </c>
@@ -4221,7 +4338,9 @@
       <c r="J18" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="25"/>
+      <c r="K18" s="25" t="s">
+        <v>160</v>
+      </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
@@ -4257,7 +4376,9 @@
       <c r="J19" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K19" s="25"/>
+      <c r="K19" s="25" t="s">
+        <v>159</v>
+      </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
@@ -4270,7 +4391,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
+    <row r="20" spans="1:20" ht="45" customHeight="1" thickBot="1">
       <c r="A20" s="20">
         <v>66</v>
       </c>
@@ -4293,7 +4414,9 @@
       <c r="J20" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K20" s="25"/>
+      <c r="K20" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
@@ -4329,7 +4452,9 @@
       <c r="J21" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K21" s="25"/>
+      <c r="K21" s="25" t="s">
+        <v>162</v>
+      </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
@@ -4365,7 +4490,9 @@
       <c r="J22" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K22" s="25"/>
+      <c r="K22" s="25" t="s">
+        <v>163</v>
+      </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
@@ -4401,7 +4528,9 @@
       <c r="J23" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K23" s="25"/>
+      <c r="K23" s="25" t="s">
+        <v>164</v>
+      </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
@@ -4437,7 +4566,9 @@
       <c r="J24" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K24" s="25"/>
+      <c r="K24" s="25" t="s">
+        <v>165</v>
+      </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
       <c r="N24" s="25"/>
@@ -4473,7 +4604,9 @@
       <c r="J25" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="25"/>
+      <c r="K25" s="25" t="s">
+        <v>166</v>
+      </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
@@ -4509,7 +4642,9 @@
       <c r="J26" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K26" s="25"/>
+      <c r="K26" s="25" t="s">
+        <v>166</v>
+      </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
@@ -4545,7 +4680,9 @@
       <c r="J27" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="25"/>
+      <c r="K27" s="25" t="s">
+        <v>167</v>
+      </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
       <c r="N27" s="25"/>
@@ -4581,7 +4718,9 @@
       <c r="J28" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="K28" s="25"/>
+      <c r="K28" s="25" t="s">
+        <v>166</v>
+      </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
       <c r="N28" s="25"/>
@@ -9001,7 +9140,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
valorizzazione colonne O e P per gli ID 29 e 37
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/V.6.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/V.6.0.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.9\condivisa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fse\it-fse-accreditamento\GATEWAY\A1#111CIDITECHSRLXX\Ciditech\Point\V.6.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A172891-BD8F-4CCC-8A07-3A078CCA9010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19C9E1A-2C1D-4C99-B7E4-04A889E6CE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="870" windowWidth="23910" windowHeight="14895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="174">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -785,6 +785,9 @@
   </si>
   <si>
     <t>Campo token JWT non valido: Il campo action_id non è corretto</t>
+  </si>
+  <si>
+    <t>il campo deve essere valorizzato correttamente; viene modificata di conseguenza la configurazione</t>
   </si>
 </sst>
 </file>
@@ -1222,6 +1225,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1244,12 +1253,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3712,10 +3715,10 @@
   <dimension ref="A1:T627"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3756,14 +3759,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="40"/>
+      <c r="D2" s="42"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3781,14 +3784,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3806,12 +3809,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="47" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3830,12 +3833,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="40"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3853,8 +3856,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4151,22 +4154,26 @@
       <c r="I14" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="J14" s="48" t="s">
+      <c r="J14" s="35" t="s">
         <v>54</v>
       </c>
       <c r="K14" s="25"/>
-      <c r="L14" s="48" t="s">
+      <c r="L14" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="48" t="s">
+      <c r="M14" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="48" t="s">
+      <c r="N14" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="48" t="s">
+      <c r="O14" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q14" s="35" t="s">
         <v>108</v>
       </c>
       <c r="R14" s="26"/>
@@ -4188,7 +4195,7 @@
       <c r="D15" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="49" t="s">
+      <c r="E15" s="36" t="s">
         <v>129</v>
       </c>
       <c r="F15" s="23">
@@ -4203,22 +4210,26 @@
       <c r="I15" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="J15" s="48" t="s">
+      <c r="J15" s="35" t="s">
         <v>54</v>
       </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="48" t="s">
+      <c r="M15" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="48" t="s">
+      <c r="N15" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="48" t="s">
+      <c r="O15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q15" s="35" t="s">
         <v>108</v>
       </c>
       <c r="R15" s="26"/>
@@ -4266,7 +4277,7 @@
       <c r="P16" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="Q16" s="48" t="s">
+      <c r="Q16" s="35" t="s">
         <v>108</v>
       </c>
       <c r="R16" s="26" t="s">

</xml_diff>

<commit_message>
fix vendorid-version in XLSX
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/V.6.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/V.6.0.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fse\it-fse-accreditamento\GATEWAY\A1#111CIDITECHSRLXX\Ciditech\Point\V.6.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19C9E1A-2C1D-4C99-B7E4-04A889E6CE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91962C50-50D4-463F-B6E7-0F9929FEFDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="870" windowWidth="23910" windowHeight="14895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4485" yWindow="105" windowWidth="19290" windowHeight="14895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -493,15 +493,6 @@
     <t>CIDITECH</t>
   </si>
   <si>
-    <t>subject_application_id: POINT</t>
-  </si>
-  <si>
-    <t>subject_application_vendor: CIDITECH</t>
-  </si>
-  <si>
-    <t>subject_application_version: 6.0.0</t>
-  </si>
-  <si>
     <t>9b505ceff6d71653</t>
   </si>
   <si>
@@ -788,6 +779,15 @@
   </si>
   <si>
     <t>il campo deve essere valorizzato correttamente; viene modificata di conseguenza la configurazione</t>
+  </si>
+  <si>
+    <t>subject_application_id: Point</t>
+  </si>
+  <si>
+    <t>subject_application_vendor: Ciditech</t>
+  </si>
+  <si>
+    <t>subject_application_version: V.6.0.0</t>
   </si>
 </sst>
 </file>
@@ -3715,10 +3715,10 @@
   <dimension ref="A1:T627"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="49" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="D3" s="40"/>
       <c r="F3" s="12"/>
@@ -3812,7 +3812,7 @@
       <c r="A4" s="45"/>
       <c r="B4" s="46"/>
       <c r="C4" s="49" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="4"/>
@@ -3836,7 +3836,7 @@
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
       <c r="C5" s="49" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="D5" s="40"/>
       <c r="F5" s="12"/>
@@ -3985,10 +3985,10 @@
         <v>47</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -3998,7 +3998,7 @@
         <v>110</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
@@ -4023,10 +4023,10 @@
         <v>47</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -4036,7 +4036,7 @@
         <v>110</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -4061,10 +4061,10 @@
         <v>47</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -4074,7 +4074,7 @@
         <v>110</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
@@ -4099,10 +4099,10 @@
         <v>47</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -4112,7 +4112,7 @@
         <v>110</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -4137,10 +4137,10 @@
         <v>47</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F14" s="23">
         <v>45189</v>
@@ -4149,10 +4149,10 @@
         <v>45189.352951388886</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J14" s="35" t="s">
         <v>54</v>
@@ -4165,13 +4165,13 @@
         <v>54</v>
       </c>
       <c r="N14" s="35" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="O14" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q14" s="35" t="s">
         <v>108</v>
@@ -4179,7 +4179,7 @@
       <c r="R14" s="26"/>
       <c r="S14" s="27"/>
       <c r="T14" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="102.75" customHeight="1" thickBot="1">
@@ -4193,10 +4193,10 @@
         <v>47</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F15" s="23">
         <v>45189</v>
@@ -4205,10 +4205,10 @@
         <v>45189.356828703705</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J15" s="35" t="s">
         <v>54</v>
@@ -4221,13 +4221,13 @@
         <v>54</v>
       </c>
       <c r="N15" s="35" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q15" s="35" t="s">
         <v>108</v>
@@ -4235,7 +4235,7 @@
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
       <c r="T15" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="122.25" customHeight="1" thickBot="1">
@@ -4249,10 +4249,10 @@
         <v>47</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -4269,13 +4269,13 @@
         <v>54</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O16" s="25" t="s">
         <v>110</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q16" s="35" t="s">
         <v>108</v>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="S16" s="27"/>
       <c r="T16" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4299,10 +4299,10 @@
         <v>47</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -4312,7 +4312,7 @@
         <v>110</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -4323,7 +4323,7 @@
       <c r="R17" s="26"/>
       <c r="S17" s="27"/>
       <c r="T17" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="30" customHeight="1" thickBot="1">
@@ -4337,10 +4337,10 @@
         <v>47</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -4350,7 +4350,7 @@
         <v>110</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -4361,7 +4361,7 @@
       <c r="R18" s="26"/>
       <c r="S18" s="27"/>
       <c r="T18" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4375,10 +4375,10 @@
         <v>47</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -4388,7 +4388,7 @@
         <v>110</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
@@ -4399,7 +4399,7 @@
       <c r="R19" s="26"/>
       <c r="S19" s="27"/>
       <c r="T19" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="45" customHeight="1" thickBot="1">
@@ -4413,10 +4413,10 @@
         <v>47</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
@@ -4426,7 +4426,7 @@
         <v>110</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -4437,7 +4437,7 @@
       <c r="R20" s="26"/>
       <c r="S20" s="27"/>
       <c r="T20" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4451,10 +4451,10 @@
         <v>47</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="24"/>
@@ -4464,7 +4464,7 @@
         <v>110</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -4475,7 +4475,7 @@
       <c r="R21" s="26"/>
       <c r="S21" s="27"/>
       <c r="T21" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4489,10 +4489,10 @@
         <v>47</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F22" s="23"/>
       <c r="G22" s="24"/>
@@ -4502,7 +4502,7 @@
         <v>110</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -4513,7 +4513,7 @@
       <c r="R22" s="26"/>
       <c r="S22" s="27"/>
       <c r="T22" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4527,10 +4527,10 @@
         <v>47</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F23" s="23"/>
       <c r="G23" s="24"/>
@@ -4540,7 +4540,7 @@
         <v>110</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -4551,7 +4551,7 @@
       <c r="R23" s="26"/>
       <c r="S23" s="27"/>
       <c r="T23" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4565,10 +4565,10 @@
         <v>47</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="24"/>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -4589,7 +4589,7 @@
       <c r="R24" s="26"/>
       <c r="S24" s="27"/>
       <c r="T24" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4603,10 +4603,10 @@
         <v>47</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="24"/>
@@ -4616,7 +4616,7 @@
         <v>110</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -4627,7 +4627,7 @@
       <c r="R25" s="26"/>
       <c r="S25" s="27"/>
       <c r="T25" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4641,10 +4641,10 @@
         <v>47</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="24"/>
@@ -4654,7 +4654,7 @@
         <v>110</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -4665,7 +4665,7 @@
       <c r="R26" s="26"/>
       <c r="S26" s="27"/>
       <c r="T26" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4679,10 +4679,10 @@
         <v>47</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
@@ -4692,7 +4692,7 @@
         <v>110</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -4703,7 +4703,7 @@
       <c r="R27" s="26"/>
       <c r="S27" s="27"/>
       <c r="T27" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
@@ -4717,10 +4717,10 @@
         <v>47</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
@@ -4730,7 +4730,7 @@
         <v>110</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
@@ -4741,7 +4741,7 @@
       <c r="R28" s="26"/>
       <c r="S28" s="27"/>
       <c r="T28" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="14.25" customHeight="1">
@@ -4767,10 +4767,10 @@
         <v>45182.647361111114</v>
       </c>
       <c r="H29" s="33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I29" s="33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>54</v>

</xml_diff>